<commit_message>
Code tested and working correctly
</commit_message>
<xml_diff>
--- a/output/revenues.xlsx
+++ b/output/revenues.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,10 +441,15 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Release Month</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Global Box Office ($)</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Global Box Office ($)</t>
         </is>
@@ -453,157 +458,193 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Apr</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>106278816.7185185</v>
+          <t>Jan</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>14347640257</v>
+        <v>80344605.43209876</v>
+      </c>
+      <c r="D2" t="n">
+        <v>6507913040</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Aug</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>114346893.5384615</v>
+          <t>Feb</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>17838115392</v>
+        <v>119750271.5304348</v>
+      </c>
+      <c r="D3" t="n">
+        <v>13771281226</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Dec</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>259328218.655814</v>
+          <t>Mar</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>55755567011</v>
+        <v>155136539.7810219</v>
+      </c>
+      <c r="D4" t="n">
+        <v>21253705950</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Feb</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>119750271.5304348</v>
+          <t>Apr</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>13771281226</v>
+        <v>106278816.7185185</v>
+      </c>
+      <c r="D5" t="n">
+        <v>14347640257</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Jan</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>80344605.43209876</v>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>6507913040</v>
+        <v>423040095.6546763</v>
+      </c>
+      <c r="D6" t="n">
+        <v>58802573296</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Jul</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>261929486.7108434</v>
+          <t>Jun</t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>43480294794</v>
+        <v>325237427.3935484</v>
+      </c>
+      <c r="D7" t="n">
+        <v>50411801246</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Jun</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>325237427.3935484</v>
+          <t>Jul</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>50411801246</v>
+        <v>261929486.7108434</v>
+      </c>
+      <c r="D8" t="n">
+        <v>43480294794</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Mar</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>155136539.7810219</v>
+          <t>Aug</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>21253705950</v>
+        <v>114346893.5384615</v>
+      </c>
+      <c r="D9" t="n">
+        <v>17838115392</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>May</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>423040095.6546763</v>
+          <t>Sep</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>58802573296</v>
+        <v>80300568.7173913</v>
+      </c>
+      <c r="D10" t="n">
+        <v>11081478483</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Nov</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>242122733.4970414</v>
+          <t>Oct</t>
+        </is>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>40918741961</v>
+        <v>102282825.5424837</v>
+      </c>
+      <c r="D11" t="n">
+        <v>15649272308</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>Oct</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>102282825.5424837</v>
+          <t>Nov</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>15649272308</v>
+        <v>242122733.4970414</v>
+      </c>
+      <c r="D12" t="n">
+        <v>40918741961</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>Sep</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>80300568.7173913</v>
+          <t>Dec</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>11081478483</v>
+        <v>259328218.655814</v>
+      </c>
+      <c r="D13" t="n">
+        <v>55755567011</v>
       </c>
     </row>
   </sheetData>

</xml_diff>